<commit_message>
Complete first excel report
</commit_message>
<xml_diff>
--- a/app/Services/Templates/Invoice_client.xlsx
+++ b/app/Services/Templates/Invoice_client.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmer\Projects\Personal\excel-export\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmer\Projects\Order\TourCrm\tour_crm_admin\app\Services\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -146,9 +146,6 @@
 {expensesList}</t>
   </si>
   <si>
-    <t>{cityFrom} - {cityTo} flight</t>
-  </si>
-  <si>
     <t>Waived off charges of the Tour leader ({paxPrice}$+{planePrice}$)</t>
   </si>
   <si>
@@ -200,7 +197,10 @@
     <t>{tourLeadersPrice}</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>{flightInfo}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{rooming} </t>
   </si>
 </sst>
 </file>
@@ -212,7 +212,7 @@
     <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="[$€-2]\ #,##0.00_);[Red]\([$€-2]\ #,##0.00\)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,12 +337,6 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -482,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -622,15 +616,78 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -646,80 +703,14 @@
     <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,7 +749,7 @@
         <xdr:cNvPr id="8" name="Line 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D2BBB73-23BF-4306-951D-9C8CC5C2BB86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D2BBB73-23BF-4306-951D-9C8CC5C2BB86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -805,7 +796,7 @@
         <xdr:cNvPr id="11" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2624C28-77B8-4FA4-8B1F-51F58A16934E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2624C28-77B8-4FA4-8B1F-51F58A16934E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1277,7 +1268,7 @@
   <dimension ref="A1:AP59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1521,11 +1512,11 @@
       <c r="A6" s="8"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="77"/>
-      <c r="F6" s="77"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
       <c r="G6" s="9" t="s">
         <v>29</v>
       </c>
@@ -1610,21 +1601,21 @@
       <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="87" t="s">
+      <c r="H8" s="55" t="s">
         <v>3</v>
       </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="78" t="s">
+      <c r="J8" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="78"/>
+      <c r="K8" s="59"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1661,19 +1652,19 @@
       <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="87" t="s">
+      <c r="H9" s="55" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="9"/>
-      <c r="J9" s="81" t="s">
+      <c r="J9" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="81"/>
+      <c r="K9" s="62"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1708,19 +1699,19 @@
     <row r="10" spans="1:42" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
       <c r="G10" s="9"/>
       <c r="H10" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="9"/>
-      <c r="J10" s="82" t="s">
+      <c r="J10" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="K10" s="82"/>
+      <c r="K10" s="63"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1757,19 +1748,19 @@
       <c r="B11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9" t="s">
         <v>16</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="57" t="s">
+      <c r="J11" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="65"/>
+      <c r="K11" s="67"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1813,10 +1804,10 @@
         <v>17</v>
       </c>
       <c r="I12" s="9"/>
-      <c r="J12" s="57" t="s">
+      <c r="J12" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="57"/>
+      <c r="K12" s="66"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1853,21 +1844,21 @@
       <c r="B13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="66" t="s">
+      <c r="C13" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="9"/>
-      <c r="J13" s="85" t="s">
+      <c r="J13" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="K13" s="85"/>
+      <c r="K13" s="84"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1909,8 +1900,8 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="83"/>
-      <c r="K14" s="83"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1953,7 +1944,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="86"/>
-      <c r="K15" s="84"/>
+      <c r="K15" s="86"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -2052,13 +2043,13 @@
       <c r="G17" s="70"/>
       <c r="H17" s="70"/>
       <c r="I17" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="K17" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -2096,7 +2087,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="71" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C18" s="72"/>
       <c r="D18" s="72"/>
@@ -2105,13 +2096,13 @@
       <c r="G18" s="72"/>
       <c r="H18" s="73"/>
       <c r="I18" s="39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -2149,7 +2140,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="72"/>
       <c r="D19" s="72"/>
@@ -2158,13 +2149,13 @@
       <c r="G19" s="72"/>
       <c r="H19" s="73"/>
       <c r="I19" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="K19" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -2211,7 +2202,7 @@
         <v>24</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -2249,7 +2240,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="72"/>
       <c r="D21" s="72"/>
@@ -2258,13 +2249,13 @@
       <c r="G21" s="72"/>
       <c r="H21" s="73"/>
       <c r="I21" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>48</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -2311,7 +2302,7 @@
         <v>25</v>
       </c>
       <c r="K22" s="51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -2350,14 +2341,14 @@
       <c r="C23" s="43"/>
       <c r="D23" s="44"/>
       <c r="E23" s="45"/>
-      <c r="F23" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="63"/>
+      <c r="F23" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -2738,18 +2729,18 @@
     </row>
     <row r="32" spans="1:42" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="36"/>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="79"/>
+      <c r="E32" s="79"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="79"/>
+      <c r="K32" s="79"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
@@ -2783,17 +2774,17 @@
     </row>
     <row r="33" spans="1:42" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27"/>
-      <c r="B33" s="59" t="s">
+      <c r="B33" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="56"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="81"/>
+      <c r="G33" s="81"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="78"/>
       <c r="K33" s="27"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -2828,17 +2819,17 @@
     </row>
     <row r="34" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A34" s="27"/>
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="56"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="78"/>
       <c r="K34" s="27"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2873,15 +2864,15 @@
     </row>
     <row r="35" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A35" s="27"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="56"/>
+      <c r="B35" s="77"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="78"/>
       <c r="K35" s="27"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -2916,15 +2907,15 @@
     </row>
     <row r="36" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A36" s="27"/>
-      <c r="B36" s="55"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="56"/>
+      <c r="B36" s="77"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="77"/>
+      <c r="J36" s="78"/>
       <c r="K36" s="27"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
@@ -2959,15 +2950,15 @@
     </row>
     <row r="37" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A37" s="27"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="56"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="78"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="78"/>
+      <c r="F37" s="78"/>
+      <c r="G37" s="78"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="77"/>
+      <c r="J37" s="78"/>
       <c r="K37" s="27"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -3002,15 +2993,15 @@
     </row>
     <row r="38" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A38" s="27"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="56"/>
+      <c r="B38" s="77"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="78"/>
+      <c r="H38" s="78"/>
+      <c r="I38" s="77"/>
+      <c r="J38" s="78"/>
       <c r="K38" s="27"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -3045,15 +3036,15 @@
     </row>
     <row r="39" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A39" s="27"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="56"/>
+      <c r="B39" s="77"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="78"/>
+      <c r="H39" s="78"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="78"/>
       <c r="K39" s="27"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
@@ -3887,23 +3878,7 @@
       <c r="AL59" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C9:F10"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="F23:K23"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="A20:I20"/>
+  <mergeCells count="33">
     <mergeCell ref="B39:H39"/>
     <mergeCell ref="I39:J39"/>
     <mergeCell ref="J12:K12"/>
@@ -3920,6 +3895,23 @@
     <mergeCell ref="I34:J34"/>
     <mergeCell ref="B35:H35"/>
     <mergeCell ref="I35:J35"/>
+    <mergeCell ref="F23:K23"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="J13:K15"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C9:F10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Промежуточный итог" error="Серые ячейки содержат формулы, автоматически вычисляемые Excel. НЕ нужно вводить в них данные." promptTitle="Промежуточный итог" sqref="K28:K31 K33:K39">

</xml_diff>

<commit_message>
Excel total price for client
</commit_message>
<xml_diff>
--- a/app/Services/Templates/Invoice_client.xlsx
+++ b/app/Services/Templates/Invoice_client.xlsx
@@ -136,59 +136,59 @@
     <t>{departureDate}</t>
   </si>
   <si>
-    <t>Uzbekistan 10D/9N tour by TK flights
+    <t>{paxPrice}</t>
+  </si>
+  <si>
+    <t>{pax}</t>
+  </si>
+  <si>
+    <t>{paxPriceTotal}</t>
+  </si>
+  <si>
+    <t>{extraPrice}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {extraPax}</t>
+  </si>
+  <si>
+    <t>{extraPriceTotal}</t>
+  </si>
+  <si>
+    <t>{priceTotal}</t>
+  </si>
+  <si>
+    <t>{tourLeadersCount}</t>
+  </si>
+  <si>
+    <t>{tourLeaderPriceTotal}</t>
+  </si>
+  <si>
+    <t>{dueTotal}</t>
+  </si>
+  <si>
+    <t>{dueTotalWithWords} USD</t>
+  </si>
+  <si>
+    <t>{tourLeadersPrice}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{rooming} </t>
+  </si>
+  <si>
+    <t>{company}</t>
+  </si>
+  <si>
+    <t>{package}</t>
+  </si>
+  <si>
+    <t>{extraNames}</t>
+  </si>
+  <si>
+    <t>Waived off charges of the Tour leader ({paxPrice}$)</t>
+  </si>
+  <si>
+    <t>{package}
 {expensesList}</t>
-  </si>
-  <si>
-    <t>{paxPrice}</t>
-  </si>
-  <si>
-    <t>{pax}</t>
-  </si>
-  <si>
-    <t>{paxPriceTotal}</t>
-  </si>
-  <si>
-    <t>{extraPrice}</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> {extraPax}</t>
-  </si>
-  <si>
-    <t>{extraPriceTotal}</t>
-  </si>
-  <si>
-    <t>{priceTotal}</t>
-  </si>
-  <si>
-    <t>{tourLeadersCount}</t>
-  </si>
-  <si>
-    <t>{tourLeaderPriceTotal}</t>
-  </si>
-  <si>
-    <t>{dueTotal}</t>
-  </si>
-  <si>
-    <t>{dueTotalWithWords} USD</t>
-  </si>
-  <si>
-    <t>{tourLeadersPrice}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{rooming} </t>
-  </si>
-  <si>
-    <t>{company}</t>
-  </si>
-  <si>
-    <t>{package}</t>
-  </si>
-  <si>
-    <t>{extraNames}</t>
-  </si>
-  <si>
-    <t>Waived off charges of the Tour leader ({paxPrice}$)</t>
   </si>
 </sst>
 </file>
@@ -607,15 +607,84 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -630,75 +699,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,7 +737,7 @@
         <xdr:cNvPr id="8" name="Line 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D2BBB73-23BF-4306-951D-9C8CC5C2BB86}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D2BBB73-23BF-4306-951D-9C8CC5C2BB86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -784,7 +784,7 @@
         <xdr:cNvPr id="11" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B2624C28-77B8-4FA4-8B1F-51F58A16934E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2624C28-77B8-4FA4-8B1F-51F58A16934E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:H18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1500,11 +1500,11 @@
       <c r="A6" s="8"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
       <c r="G6" s="9" t="s">
         <v>27</v>
       </c>
@@ -1589,21 +1589,21 @@
       <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
+      <c r="C8" s="67" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
       <c r="G8" s="9"/>
       <c r="H8" s="55" t="s">
         <v>3</v>
       </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="59"/>
+      <c r="K8" s="82"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1640,19 +1640,19 @@
       <c r="B9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
       <c r="G9" s="9"/>
       <c r="H9" s="55" t="s">
         <v>5</v>
       </c>
       <c r="I9" s="9"/>
-      <c r="J9" s="62" t="s">
+      <c r="J9" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="62"/>
+      <c r="K9" s="85"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1687,19 +1687,19 @@
     <row r="10" spans="1:42" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
       <c r="G10" s="9"/>
       <c r="H10" s="12" t="s">
         <v>6</v>
       </c>
       <c r="I10" s="9"/>
-      <c r="J10" s="63" t="s">
+      <c r="J10" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="63"/>
+      <c r="K10" s="86"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1745,10 +1745,10 @@
         <v>16</v>
       </c>
       <c r="I11" s="9"/>
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="67"/>
+      <c r="K11" s="66"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1792,10 +1792,10 @@
         <v>17</v>
       </c>
       <c r="I12" s="9"/>
-      <c r="J12" s="66" t="s">
+      <c r="J12" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="66"/>
+      <c r="K12" s="58"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1832,21 +1832,21 @@
       <c r="B13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
+      <c r="C13" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="9"/>
-      <c r="J13" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="77"/>
+      <c r="J13" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="78"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1888,8 +1888,8 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -1931,8 +1931,8 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="80"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1968,15 +1968,15 @@
       <c r="A16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
       <c r="I16" s="38" t="s">
         <v>12</v>
       </c>
@@ -2021,23 +2021,23 @@
       <c r="A17" s="52">
         <v>1</v>
       </c>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="39" t="s">
+      <c r="J17" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="K17" s="15" t="s">
         <v>34</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>35</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -2074,23 +2074,23 @@
       <c r="A18" s="53">
         <v>2</v>
       </c>
-      <c r="B18" s="71" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="73"/>
+      <c r="B18" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="74"/>
       <c r="I18" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="K18" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>38</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -2124,20 +2124,20 @@
       <c r="AP18" s="4"/>
     </row>
     <row r="19" spans="1:42" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="74"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="76"/>
+      <c r="A19" s="75"/>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="77"/>
       <c r="J19" s="50" t="s">
         <v>22</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -2174,23 +2174,23 @@
       <c r="A20" s="53">
         <v>3</v>
       </c>
-      <c r="B20" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="73"/>
+      <c r="B20" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="74"/>
       <c r="I20" s="39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -2237,7 +2237,7 @@
         <v>23</v>
       </c>
       <c r="K21" s="51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -2277,7 +2277,7 @@
       <c r="D22" s="44"/>
       <c r="E22" s="45"/>
       <c r="F22" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" s="64"/>
       <c r="H22" s="64"/>
@@ -2664,18 +2664,18 @@
     </row>
     <row r="31" spans="1:42" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="36"/>
-      <c r="B31" s="82" t="s">
+      <c r="B31" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="82"/>
-      <c r="D31" s="82"/>
-      <c r="E31" s="82"/>
-      <c r="F31" s="82"/>
-      <c r="G31" s="82"/>
-      <c r="H31" s="82"/>
-      <c r="I31" s="82"/>
-      <c r="J31" s="82"/>
-      <c r="K31" s="82"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
@@ -2709,17 +2709,17 @@
     </row>
     <row r="32" spans="1:42" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27"/>
-      <c r="B32" s="83" t="s">
+      <c r="B32" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="84"/>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
-      <c r="G32" s="84"/>
-      <c r="H32" s="84"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="81"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="57"/>
       <c r="K32" s="27"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
@@ -2754,17 +2754,17 @@
     </row>
     <row r="33" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A33" s="27"/>
-      <c r="B33" s="85" t="s">
+      <c r="B33" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="86"/>
-      <c r="H33" s="86"/>
-      <c r="I33" s="80"/>
-      <c r="J33" s="81"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="57"/>
       <c r="K33" s="27"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
@@ -2799,15 +2799,15 @@
     </row>
     <row r="34" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A34" s="27"/>
-      <c r="B34" s="80"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="80"/>
-      <c r="J34" s="81"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="56"/>
+      <c r="J34" s="57"/>
       <c r="K34" s="27"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
@@ -2842,15 +2842,15 @@
     </row>
     <row r="35" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A35" s="27"/>
-      <c r="B35" s="80"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="81"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="57"/>
       <c r="K35" s="27"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -2885,15 +2885,15 @@
     </row>
     <row r="36" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A36" s="27"/>
-      <c r="B36" s="80"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="81"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="57"/>
       <c r="K36" s="27"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
@@ -2928,15 +2928,15 @@
     </row>
     <row r="37" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A37" s="27"/>
-      <c r="B37" s="80"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="81"/>
-      <c r="I37" s="80"/>
-      <c r="J37" s="81"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="57"/>
       <c r="K37" s="27"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -2971,15 +2971,15 @@
     </row>
     <row r="38" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A38" s="27"/>
-      <c r="B38" s="80"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
-      <c r="G38" s="81"/>
-      <c r="H38" s="81"/>
-      <c r="I38" s="80"/>
-      <c r="J38" s="81"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="57"/>
       <c r="K38" s="27"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
@@ -3814,6 +3814,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="C9:F10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="J13:K15"/>
     <mergeCell ref="B38:H38"/>
     <mergeCell ref="I38:J38"/>
     <mergeCell ref="J12:K12"/>
@@ -3830,22 +3846,6 @@
     <mergeCell ref="I33:J33"/>
     <mergeCell ref="B34:H34"/>
     <mergeCell ref="I34:J34"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="J13:K15"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="C9:F10"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="textLength" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Промежуточный итог" error="Серые ячейки содержат формулы, автоматически вычисляемые Excel. НЕ нужно вводить в них данные." promptTitle="Промежуточный итог" sqref="K27:K30 K32:K38">

</xml_diff>